<commit_message>
Updated IND model - 2025-07-31 23:07
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/SuppXLS/scen_tsparameters_ts_336.xlsx
+++ b/VerveStacks_IND/SuppXLS/scen_tsparameters_ts_336.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_IND\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD72F745-7CA4-4F8A-BBA9-C4EF0D7FC99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE65D9C1-84FB-4E33-87F4-6BC9806B7A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -1569,10 +1569,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>m01ah08,m02ah08,m02ah14,m03ah17,m05ah17,m06ah15,m07ah15,m08ah11,m09ah07,m09ah14,m01ah15,m01ah18,m01b0121h14,m02ah07,m04ah08,m04ah14,m05ah07,m05ah13,m07c0716h07,m07c0716h15,m08ah18,m10ah18,m12ah11,m03ah16,m04ah18,m05ah10,m07ah17,m07c0716h09,m12ah07,m01ah14,m01b0121h15,m01b0121h17,m02ah09,m02ah10,m02ah12,m03ah08,m03ah09,m05ah14,m07c0716h16,m11ah08,m11ah15,m12ah17,m01b0121h07,m03ah13,m07ah10,m07ah18,m07c0716h14,m08ah08,m08ah10,m11ah14,m12ah08,m01ah17,m02ah13,m05ah16,m06ah14,m07c0716h11,m09ah11,m09ah18,m10ah09,m10ah13,m11ah16,m12ah15,m01b0121h13,m03ah14,m04ah09,m04ah15,m06ah08,m07c0716h08,m08ah13,m08ah14,m09ah08,m09ah09,m09ah16,m10ah07,m10ah16,m10ah17,m12ah09,m01ah12,m01ah13,m01b0121h18,m04ah10,m04ah16,m05ah08,m06ah13,m07ah13,m09ah12,m10ah10,m10ah11,m11ah07,m01ah09,m01b0121h09,m01b0121h16,m02ah18,m03ah18,m05ah12,m05ah18,m07c0716h18,m08ah07,m10ah15,m11ah12,m12ah18,m01b0121h12,m03ah07,m05ah11,m06ah07,m06ah10,m06ah18,m07ah08,m08ah17,m09ah17,m10ah08,m01ah10,m01ah16,m03ah10,m03ah11,m04ah07,m06ah17,m08ah12,m11ah17,m12ah10,m12ah16,m01b0121h08,m02ah15,m04ah17,m07ah09,m07c0716h17,m10ah12,m10ah14,m11ah09,m11ah13,m03ah15,m04ah13,m06ah09,m07ah07,m07ah16,m09ah13,m01ah07,m02ah11,m05ah09,m05ah15,m07ah12,m09ah10,m11ah11,m11ah18,m12ah14,m01ah11,m01b0121h10,m03ah12,m04ah11,m04ah12,m06ah12,m06ah16,m07c0716h10,m07c0716h12,m08ah09,m09ah15,m11ah10,m12ah12,m01b0121h11,m02ah16,m02ah17,m06ah11,m07ah11,m07ah14,m07c0716h13,m08ah15,m08ah16,m12ah13</t>
-  </si>
-  <si>
-    <t>m01b0121h22,m03ah22,m04ah05,m06ah04,m06ah19,m06ah20,m07c0716h04,m07c0716h24,m09ah20,m11ah19,m12ah22,m02ah03,m02ah04,m02ah22,m07ah01,m07ah20,m07c0716h01,m09ah22,m09ah24,m10ah21,m11ah02,m12ah20,m12ah23,m02ah02,m02ah19,m02ah21,m03ah20,m07ah19,m07ah23,m07c0716h20,m08ah19,m08ah22,m09ah06,m10ah20,m11ah06,m11ah21,m01ah02,m01ah19,m01ah22,m01b0121h23,m02ah05,m03ah01,m04ah23,m05ah04,m08ah04,m09ah01,m12ah06,m12ah19,m01ah03,m01ah21,m01b0121h19,m01b0121h24,m04ah24,m05ah21,m05ah24,m07ah02,m09ah23,m10ah04,m10ah22,m10ah24,m11ah03,m01b0121h03,m02ah20,m03ah23,m04ah22,m07c0716h22,m08ah01,m08ah23,m10ah02,m11ah01,m11ah04,m01ah20,m03ah05,m04ah03,m04ah19,m04ah21,m05ah23,m07ah24,m07c0716h03,m07c0716h21,m11ah24,m01ah04,m03ah04,m04ah20,m06ah05,m09ah19,m01b0121h02,m01b0121h05,m01b0121h20,m06ah03,m07ah04,m07c0716h19,m08ah02,m08ah03,m08ah21,m09ah05,m11ah05,m12ah21,m01ah01,m01ah05,m02ah23,m04ah01,m04ah04,m06ah02,m07ah06,m07c0716h02,m07c0716h23,m09ah02,m09ah04,m10ah05,m10ah23,m11ah20,m11ah23,m01b0121h04,m01b0121h06,m01b0121h21,m03ah06,m03ah21,m04ah02,m05ah01,m05ah06,m07c0716h06,m10ah06,m10ah19,m12ah01,m01ah23,m03ah02,m03ah24,m06ah24,m07ah05,m09ah03,m11ah22,m12ah24,m02ah01,m02ah24,m03ah19,m05ah02,m05ah19,m06ah21,m07c0716h05,m08ah24,m12ah03,m01ah06,m01b0121h01,m02ah06,m03ah03,m04ah06,m05ah03,m05ah20,m06ah01,m06ah23,m07ah22,m09ah21,m12ah04,m07ah03,m07ah21,m10ah03,m12ah05,m01ah24,m05ah05,m05ah22,m06ah06,m06ah22,m08ah05,m08ah06,m08ah20,m10ah01,m12ah02</t>
+    <t>m01ah11,m01b0121h10,m03ah12,m04ah11,m04ah12,m06ah12,m06ah16,m07c0716h10,m07c0716h12,m08ah09,m09ah15,m11ah10,m12ah12,m01b0121h13,m03ah14,m04ah09,m04ah15,m06ah08,m07c0716h08,m08ah13,m08ah14,m09ah08,m09ah09,m09ah16,m10ah07,m10ah16,m10ah17,m12ah09,m01b0121h07,m03ah13,m07ah10,m07ah18,m07c0716h14,m08ah08,m08ah10,m11ah14,m12ah08,m01ah15,m01ah18,m01b0121h14,m02ah07,m04ah08,m04ah14,m05ah07,m05ah13,m07c0716h07,m07c0716h15,m08ah18,m10ah18,m12ah11,m01ah07,m02ah11,m05ah09,m05ah15,m07ah12,m09ah10,m11ah11,m11ah18,m12ah14,m01ah12,m01ah13,m01b0121h18,m04ah10,m04ah16,m05ah08,m06ah13,m07ah13,m09ah12,m10ah10,m10ah11,m11ah07,m01b0121h12,m03ah07,m05ah11,m06ah07,m06ah10,m06ah18,m07ah08,m08ah17,m09ah17,m10ah08,m01ah14,m01b0121h15,m01b0121h17,m02ah09,m02ah10,m02ah12,m03ah08,m03ah09,m05ah14,m07c0716h16,m11ah08,m11ah15,m12ah17,m03ah16,m04ah18,m05ah10,m07ah17,m07c0716h09,m12ah07,m01ah17,m02ah13,m05ah16,m06ah14,m07c0716h11,m09ah11,m09ah18,m10ah09,m10ah13,m11ah16,m12ah15,m01ah10,m01ah16,m03ah10,m03ah11,m04ah07,m06ah17,m08ah12,m11ah17,m12ah10,m12ah16,m01ah09,m01b0121h09,m01b0121h16,m02ah18,m03ah18,m05ah12,m05ah18,m07c0716h18,m08ah07,m10ah15,m11ah12,m12ah18,m01b0121h08,m02ah15,m04ah17,m07ah09,m07c0716h17,m10ah12,m10ah14,m11ah09,m11ah13,m03ah15,m04ah13,m06ah09,m07ah07,m07ah16,m09ah13,m01ah08,m02ah08,m02ah14,m03ah17,m05ah17,m06ah15,m07ah15,m08ah11,m09ah07,m09ah14,m01b0121h11,m02ah16,m02ah17,m06ah11,m07ah11,m07ah14,m07c0716h13,m08ah15,m08ah16,m12ah13</t>
+  </si>
+  <si>
+    <t>m07ah03,m07ah21,m10ah03,m12ah05,m01ah20,m03ah05,m04ah03,m04ah19,m04ah21,m05ah23,m07ah24,m07c0716h03,m07c0716h21,m11ah24,m01ah03,m01ah21,m01b0121h19,m01b0121h24,m04ah24,m05ah21,m05ah24,m07ah02,m09ah23,m10ah04,m10ah22,m10ah24,m11ah03,m02ah03,m02ah04,m02ah22,m07ah01,m07ah20,m07c0716h01,m09ah22,m09ah24,m10ah21,m11ah02,m12ah20,m12ah23,m01ah06,m01b0121h01,m02ah06,m03ah03,m04ah06,m05ah03,m05ah20,m06ah01,m06ah23,m07ah22,m09ah21,m12ah04,m01ah04,m03ah04,m04ah20,m06ah05,m09ah19,m01ah01,m01ah05,m02ah23,m04ah01,m04ah04,m06ah02,m07ah06,m07c0716h02,m07c0716h23,m09ah02,m09ah04,m10ah05,m10ah23,m11ah20,m11ah23,m01ah02,m01ah19,m01ah22,m01b0121h23,m02ah05,m03ah01,m04ah23,m05ah04,m08ah04,m09ah01,m12ah06,m12ah19,m02ah02,m02ah19,m02ah21,m03ah20,m07ah19,m07ah23,m07c0716h20,m08ah19,m08ah22,m09ah06,m10ah20,m11ah06,m11ah21,m01b0121h03,m02ah20,m03ah23,m04ah22,m07c0716h22,m08ah01,m08ah23,m10ah02,m11ah01,m11ah04,m01b0121h04,m01b0121h06,m01b0121h21,m03ah06,m03ah21,m04ah02,m05ah01,m05ah06,m07c0716h06,m10ah06,m10ah19,m12ah01,m01b0121h02,m01b0121h05,m01b0121h20,m06ah03,m07ah04,m07c0716h19,m08ah02,m08ah03,m08ah21,m09ah05,m11ah05,m12ah21,m01ah23,m03ah02,m03ah24,m06ah24,m07ah05,m09ah03,m11ah22,m12ah24,m02ah01,m02ah24,m03ah19,m05ah02,m05ah19,m06ah21,m07c0716h05,m08ah24,m12ah03,m01b0121h22,m03ah22,m04ah05,m06ah04,m06ah19,m06ah20,m07c0716h04,m07c0716h24,m09ah20,m11ah19,m12ah22,m01ah24,m05ah05,m05ah22,m06ah06,m06ah22,m08ah05,m08ah06,m08ah20,m10ah01,m12ah02</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>m01b0121h22,m03ah22,m04ah05,m06ah04,m06ah19,m06ah20,m07c0716h04,m07c0716h24,m09ah20,m11ah19,m12ah22,m02ah03,m02ah04,m02ah22,m07ah01,m07ah20,m07c0716h01,m09ah22,m09ah24,m10ah21,m11ah02,m12ah20,m12ah23,m02ah02,m02ah19,m02ah21,m03ah20,m07ah19,m07ah23,m07c0716h20,m08ah19,m08ah22,m09ah06,m10ah20,m11ah06,m11ah21,m01ah02,m01ah19,m01ah22,m01b0121h23,m02ah05,m03ah01,m04ah23,m05ah04,m08ah04,m09ah01,m12ah06,m12ah19,m01ah03,m01ah21,m01b0121h19,m01b0121h24,m04ah24,m05ah21,m05ah24,m07ah02,m09ah23,m10ah04,m10ah22,m10ah24,m11ah03,m01b0121h03,m02ah20,m03ah23,m04ah22,m07c0716h22,m08ah01,m08ah23,m10ah02,m11ah01,m11ah04,m01ah20,m03ah05,m04ah03,m04ah19,m04ah21,m05ah23,m07ah24,m07c0716h03,m07c0716h21,m11ah24,m01ah04,m03ah04,m04ah20,m06ah05,m09ah19,m01b0121h02,m01b0121h05,m01b0121h20,m06ah03,m07ah04,m07c0716h19,m08ah02,m08ah03,m08ah21,m09ah05,m11ah05,m12ah21,m01ah01,m01ah05,m02ah23,m04ah01,m04ah04,m06ah02,m07ah06,m07c0716h02,m07c0716h23,m09ah02,m09ah04,m10ah05,m10ah23,m11ah20,m11ah23,m01b0121h04,m01b0121h06,m01b0121h21,m03ah06,m03ah21,m04ah02,m05ah01,m05ah06,m07c0716h06,m10ah06,m10ah19,m12ah01,m01ah23,m03ah02,m03ah24,m06ah24,m07ah05,m09ah03,m11ah22,m12ah24,m02ah01,m02ah24,m03ah19,m05ah02,m05ah19,m06ah21,m07c0716h05,m08ah24,m12ah03,m01ah06,m01b0121h01,m02ah06,m03ah03,m04ah06,m05ah03,m05ah20,m06ah01,m06ah23,m07ah22,m09ah21,m12ah04,m07ah03,m07ah21,m10ah03,m12ah05,m01ah24,m05ah05,m05ah22,m06ah06,m06ah22,m08ah05,m08ah06,m08ah20,m10ah01,m12ah02</v>
+        <v>m07ah03,m07ah21,m10ah03,m12ah05,m01ah20,m03ah05,m04ah03,m04ah19,m04ah21,m05ah23,m07ah24,m07c0716h03,m07c0716h21,m11ah24,m01ah03,m01ah21,m01b0121h19,m01b0121h24,m04ah24,m05ah21,m05ah24,m07ah02,m09ah23,m10ah04,m10ah22,m10ah24,m11ah03,m02ah03,m02ah04,m02ah22,m07ah01,m07ah20,m07c0716h01,m09ah22,m09ah24,m10ah21,m11ah02,m12ah20,m12ah23,m01ah06,m01b0121h01,m02ah06,m03ah03,m04ah06,m05ah03,m05ah20,m06ah01,m06ah23,m07ah22,m09ah21,m12ah04,m01ah04,m03ah04,m04ah20,m06ah05,m09ah19,m01ah01,m01ah05,m02ah23,m04ah01,m04ah04,m06ah02,m07ah06,m07c0716h02,m07c0716h23,m09ah02,m09ah04,m10ah05,m10ah23,m11ah20,m11ah23,m01ah02,m01ah19,m01ah22,m01b0121h23,m02ah05,m03ah01,m04ah23,m05ah04,m08ah04,m09ah01,m12ah06,m12ah19,m02ah02,m02ah19,m02ah21,m03ah20,m07ah19,m07ah23,m07c0716h20,m08ah19,m08ah22,m09ah06,m10ah20,m11ah06,m11ah21,m01b0121h03,m02ah20,m03ah23,m04ah22,m07c0716h22,m08ah01,m08ah23,m10ah02,m11ah01,m11ah04,m01b0121h04,m01b0121h06,m01b0121h21,m03ah06,m03ah21,m04ah02,m05ah01,m05ah06,m07c0716h06,m10ah06,m10ah19,m12ah01,m01b0121h02,m01b0121h05,m01b0121h20,m06ah03,m07ah04,m07c0716h19,m08ah02,m08ah03,m08ah21,m09ah05,m11ah05,m12ah21,m01ah23,m03ah02,m03ah24,m06ah24,m07ah05,m09ah03,m11ah22,m12ah24,m02ah01,m02ah24,m03ah19,m05ah02,m05ah19,m06ah21,m07c0716h05,m08ah24,m12ah03,m01b0121h22,m03ah22,m04ah05,m06ah04,m06ah19,m06ah20,m07c0716h04,m07c0716h24,m09ah20,m11ah19,m12ah22,m01ah24,m05ah05,m05ah22,m06ah06,m06ah22,m08ah05,m08ah06,m08ah20,m10ah01,m12ah02</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -2175,7 +2175,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>m01ah08,m02ah08,m02ah14,m03ah17,m05ah17,m06ah15,m07ah15,m08ah11,m09ah07,m09ah14,m01ah15,m01ah18,m01b0121h14,m02ah07,m04ah08,m04ah14,m05ah07,m05ah13,m07c0716h07,m07c0716h15,m08ah18,m10ah18,m12ah11,m03ah16,m04ah18,m05ah10,m07ah17,m07c0716h09,m12ah07,m01ah14,m01b0121h15,m01b0121h17,m02ah09,m02ah10,m02ah12,m03ah08,m03ah09,m05ah14,m07c0716h16,m11ah08,m11ah15,m12ah17,m01b0121h07,m03ah13,m07ah10,m07ah18,m07c0716h14,m08ah08,m08ah10,m11ah14,m12ah08,m01ah17,m02ah13,m05ah16,m06ah14,m07c0716h11,m09ah11,m09ah18,m10ah09,m10ah13,m11ah16,m12ah15,m01b0121h13,m03ah14,m04ah09,m04ah15,m06ah08,m07c0716h08,m08ah13,m08ah14,m09ah08,m09ah09,m09ah16,m10ah07,m10ah16,m10ah17,m12ah09,m01ah12,m01ah13,m01b0121h18,m04ah10,m04ah16,m05ah08,m06ah13,m07ah13,m09ah12,m10ah10,m10ah11,m11ah07,m01ah09,m01b0121h09,m01b0121h16,m02ah18,m03ah18,m05ah12,m05ah18,m07c0716h18,m08ah07,m10ah15,m11ah12,m12ah18,m01b0121h12,m03ah07,m05ah11,m06ah07,m06ah10,m06ah18,m07ah08,m08ah17,m09ah17,m10ah08,m01ah10,m01ah16,m03ah10,m03ah11,m04ah07,m06ah17,m08ah12,m11ah17,m12ah10,m12ah16,m01b0121h08,m02ah15,m04ah17,m07ah09,m07c0716h17,m10ah12,m10ah14,m11ah09,m11ah13,m03ah15,m04ah13,m06ah09,m07ah07,m07ah16,m09ah13,m01ah07,m02ah11,m05ah09,m05ah15,m07ah12,m09ah10,m11ah11,m11ah18,m12ah14,m01ah11,m01b0121h10,m03ah12,m04ah11,m04ah12,m06ah12,m06ah16,m07c0716h10,m07c0716h12,m08ah09,m09ah15,m11ah10,m12ah12,m01b0121h11,m02ah16,m02ah17,m06ah11,m07ah11,m07ah14,m07c0716h13,m08ah15,m08ah16,m12ah13</v>
+        <v>m01ah11,m01b0121h10,m03ah12,m04ah11,m04ah12,m06ah12,m06ah16,m07c0716h10,m07c0716h12,m08ah09,m09ah15,m11ah10,m12ah12,m01b0121h13,m03ah14,m04ah09,m04ah15,m06ah08,m07c0716h08,m08ah13,m08ah14,m09ah08,m09ah09,m09ah16,m10ah07,m10ah16,m10ah17,m12ah09,m01b0121h07,m03ah13,m07ah10,m07ah18,m07c0716h14,m08ah08,m08ah10,m11ah14,m12ah08,m01ah15,m01ah18,m01b0121h14,m02ah07,m04ah08,m04ah14,m05ah07,m05ah13,m07c0716h07,m07c0716h15,m08ah18,m10ah18,m12ah11,m01ah07,m02ah11,m05ah09,m05ah15,m07ah12,m09ah10,m11ah11,m11ah18,m12ah14,m01ah12,m01ah13,m01b0121h18,m04ah10,m04ah16,m05ah08,m06ah13,m07ah13,m09ah12,m10ah10,m10ah11,m11ah07,m01b0121h12,m03ah07,m05ah11,m06ah07,m06ah10,m06ah18,m07ah08,m08ah17,m09ah17,m10ah08,m01ah14,m01b0121h15,m01b0121h17,m02ah09,m02ah10,m02ah12,m03ah08,m03ah09,m05ah14,m07c0716h16,m11ah08,m11ah15,m12ah17,m03ah16,m04ah18,m05ah10,m07ah17,m07c0716h09,m12ah07,m01ah17,m02ah13,m05ah16,m06ah14,m07c0716h11,m09ah11,m09ah18,m10ah09,m10ah13,m11ah16,m12ah15,m01ah10,m01ah16,m03ah10,m03ah11,m04ah07,m06ah17,m08ah12,m11ah17,m12ah10,m12ah16,m01ah09,m01b0121h09,m01b0121h16,m02ah18,m03ah18,m05ah12,m05ah18,m07c0716h18,m08ah07,m10ah15,m11ah12,m12ah18,m01b0121h08,m02ah15,m04ah17,m07ah09,m07c0716h17,m10ah12,m10ah14,m11ah09,m11ah13,m03ah15,m04ah13,m06ah09,m07ah07,m07ah16,m09ah13,m01ah08,m02ah08,m02ah14,m03ah17,m05ah17,m06ah15,m07ah15,m08ah11,m09ah07,m09ah14,m01b0121h11,m02ah16,m02ah17,m06ah11,m07ah11,m07ah14,m07c0716h13,m08ah15,m08ah16,m12ah13</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2788,7 +2788,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD2E64F4-9C4A-4BEB-BC3B-52B88512064D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44507742-5C35-43B3-B93E-49DF17B4AC3B}">
   <dimension ref="B2:F75"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3453,7 +3453,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C5E06D-50C6-47D5-A127-D2C22EC1E943}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5995E5-6822-4863-988E-97D47EE49F28}">
   <dimension ref="B2:O339"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3532,10 +3532,10 @@
         <v>168</v>
       </c>
       <c r="M4" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="N4">
-        <v>7.9098206514146938E-2</v>
+        <v>0.1732062455001665</v>
       </c>
       <c r="O4" t="s">
         <v>516</v>
@@ -3567,10 +3567,10 @@
         <v>168</v>
       </c>
       <c r="M5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="N5">
-        <v>6.1341729440462497E-2</v>
+        <v>6.3366251517854258E-2</v>
       </c>
       <c r="O5" t="s">
         <v>516</v>
@@ -3602,10 +3602,10 @@
         <v>168</v>
       </c>
       <c r="M6" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="N6">
-        <v>0.14749352561278328</v>
+        <v>6.3185720886749258E-2</v>
       </c>
       <c r="O6" t="s">
         <v>516</v>
@@ -3637,10 +3637,10 @@
         <v>168</v>
       </c>
       <c r="M7" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="N7">
-        <v>7.0510106491580612E-2</v>
+        <v>9.8763150259512766E-2</v>
       </c>
       <c r="O7" t="s">
         <v>516</v>
@@ -3672,10 +3672,10 @@
         <v>168</v>
       </c>
       <c r="M8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="N8">
-        <v>0.17320624550016653</v>
+        <v>0.10423064937297842</v>
       </c>
       <c r="O8" t="s">
         <v>516</v>
@@ -3707,10 +3707,10 @@
         <v>168</v>
       </c>
       <c r="M9" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="N9">
-        <v>0.12151000977874252</v>
+        <v>5.6196606453970052E-2</v>
       </c>
       <c r="O9" t="s">
         <v>516</v>
@@ -3742,10 +3742,10 @@
         <v>168</v>
       </c>
       <c r="M10" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="N10">
-        <v>6.3366251517854258E-2</v>
+        <v>0.16109779817105271</v>
       </c>
       <c r="O10" t="s">
         <v>516</v>
@@ -3777,10 +3777,10 @@
         <v>168</v>
       </c>
       <c r="M11" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="N11">
-        <v>9.876315025951278E-2</v>
+        <v>0.1215100097787425</v>
       </c>
       <c r="O11" t="s">
         <v>516</v>
@@ -3812,10 +3812,10 @@
         <v>168</v>
       </c>
       <c r="M12" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="N12">
-        <v>6.3185720886749258E-2</v>
+        <v>7.0510106491580599E-2</v>
       </c>
       <c r="O12" t="s">
         <v>516</v>
@@ -3847,10 +3847,10 @@
         <v>168</v>
       </c>
       <c r="M13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N13">
-        <v>0.10423064937297843</v>
+        <v>7.909820651414691E-2</v>
       </c>
       <c r="O13" t="s">
         <v>516</v>
@@ -3882,10 +3882,10 @@
         <v>168</v>
       </c>
       <c r="M14" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="N14">
-        <v>5.6196606453970052E-2</v>
+        <v>6.134172944046249E-2</v>
       </c>
       <c r="O14" t="s">
         <v>516</v>
@@ -3917,10 +3917,10 @@
         <v>168</v>
       </c>
       <c r="M15" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="N15">
-        <v>0.16109779817105274</v>
+        <v>0.14749352561278326</v>
       </c>
       <c r="O15" t="s">
         <v>516</v>
@@ -12356,7 +12356,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC45D28-B15A-4886-ABDE-1A43F8B70892}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE1FEE0-ED70-4922-AF52-682BB07B2B0C}">
   <dimension ref="B2:O647"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>